<commit_message>
resolved firmware size issue, defined inQ (seq v4)
</commit_message>
<xml_diff>
--- a/firmware sizes.xlsx
+++ b/firmware sizes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="45">
   <si>
     <t>MQTT 3.1 disabled</t>
   </si>
@@ -112,6 +112,45 @@
   </si>
   <si>
     <t>TTGO TAUDIO</t>
+  </si>
+  <si>
+    <t>E (505) esp_image: Image length 1064448 doesn't fit in partition length 1048576</t>
+  </si>
+  <si>
+    <t>INFO</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>LOGLEVEL</t>
+  </si>
+  <si>
+    <t>E (498) esp_image: Image length 1053520 doesn't fit in partition length 1048576</t>
+  </si>
+  <si>
+    <t>NO OUTPUT</t>
+  </si>
+  <si>
+    <t>EXCESS</t>
+  </si>
+  <si>
+    <t>Fits, but prone to error</t>
+  </si>
+  <si>
+    <t>HELTEC AFTER SEVERE ACTIONS:</t>
+  </si>
+  <si>
+    <t>SET LOGGING LEVEL TO ERROR</t>
+  </si>
+  <si>
+    <t>BUT USE ERROR MESSAGES FOR DEBUGGING AT CRITICAL LOCATIONS</t>
+  </si>
+  <si>
+    <t>AND WIPE THEM AGAIN AFTER USE</t>
+  </si>
+  <si>
+    <t>53.5 kB</t>
   </si>
 </sst>
 </file>
@@ -127,7 +166,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +191,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -165,12 +210,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,673 +513,924 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B8"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2">
+        <f>1064448/1048567</f>
+        <v>1.0151454318131317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3">
+        <f>1053520/1048567</f>
+        <v>1.0047235894320534</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
-      <c r="A3" s="4">
+    <row r="8" spans="1:20">
+      <c r="A8" s="4">
         <v>1089024</v>
       </c>
-      <c r="B3" s="4">
-        <f>+LOG(A3)</f>
+      <c r="B8" s="4">
+        <f>+LOG(A8)</f>
         <v>6.03703745087856</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C8" t="s">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F8" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G8" t="s">
         <v>6</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L8" t="s">
         <v>4</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
-      <c r="G4" t="s">
+    <row r="9" spans="1:20">
+      <c r="G9" t="s">
         <v>7</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H9" t="s">
         <v>8</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I9" t="s">
         <v>9</v>
       </c>
-      <c r="J4">
+      <c r="J9">
         <v>15640</v>
       </c>
-      <c r="K4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4">
-        <f>+LOG(J4)</f>
+      <c r="K9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9">
+        <f>+LOG(J9)</f>
         <v>4.1942367487238288</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
-      <c r="G5" t="s">
+    <row r="10" spans="1:20">
+      <c r="G10" t="s">
         <v>7</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H10" t="s">
         <v>11</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I10" t="s">
         <v>9</v>
       </c>
-      <c r="J5">
+      <c r="J10">
         <v>25576</v>
       </c>
-      <c r="K5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5">
-        <f t="shared" ref="L5:L10" si="0">+LOG(J5)</f>
+      <c r="K10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L10:L15" si="0">+LOG(J10)</f>
         <v>4.4078326232636318</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
-      <c r="F6" t="s">
+    <row r="11" spans="1:20">
+      <c r="F11" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G11" t="s">
         <v>13</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H11" t="s">
         <v>14</v>
       </c>
-      <c r="J6">
+      <c r="J11">
         <v>41216</v>
       </c>
-      <c r="K6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L6">
+      <c r="K11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11">
         <f t="shared" si="0"/>
         <v>4.6150658413436991</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N11" t="s">
         <v>15</v>
       </c>
-      <c r="O6">
+      <c r="O11">
         <v>83364</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P11" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="Q11" s="1">
         <v>0.33100000000000002</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R11" t="s">
         <v>17</v>
       </c>
-      <c r="S6">
-        <f>+LOG(O6)</f>
+      <c r="S11">
+        <f>+LOG(O11)</f>
         <v>4.9209785449219803</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
-      <c r="F7" t="s">
+    <row r="12" spans="1:20">
+      <c r="F12" t="s">
         <v>12</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G12" t="s">
         <v>13</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H12" t="s">
         <v>18</v>
       </c>
-      <c r="J7">
+      <c r="J12">
         <v>114907</v>
       </c>
-      <c r="K7" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7">
+      <c r="K12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12">
         <f t="shared" si="0"/>
         <v>5.0603464862058916</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N12" t="s">
         <v>15</v>
       </c>
-      <c r="O7">
+      <c r="O12">
         <v>16165</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P12" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="Q12" s="1">
         <v>0.877</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R12" t="s">
         <v>17</v>
       </c>
-      <c r="S7">
-        <f>+LOG(O7)</f>
+      <c r="S12">
+        <f>+LOG(O12)</f>
         <v>4.208575708947575</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
-      <c r="G8" t="s">
+    <row r="13" spans="1:20">
+      <c r="G13" t="s">
         <v>19</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H13" t="s">
         <v>20</v>
       </c>
-      <c r="J8">
+      <c r="J13">
         <v>599399</v>
       </c>
-      <c r="K8" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8">
+      <c r="K13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13">
         <f t="shared" si="0"/>
         <v>5.7777160140603367</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
-      <c r="G9" t="s">
+    <row r="14" spans="1:20">
+      <c r="G14" t="s">
         <v>19</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H14" t="s">
         <v>21</v>
       </c>
-      <c r="J9">
+      <c r="J14">
         <v>108032</v>
       </c>
-      <c r="K9" t="s">
-        <v>10</v>
-      </c>
-      <c r="L9">
+      <c r="K14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="0"/>
         <v>5.0335524162735235</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
-      <c r="F10" t="s">
+    <row r="15" spans="1:20">
+      <c r="F15" t="s">
         <v>5</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G15" t="s">
         <v>22</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H15" t="s">
         <v>23</v>
       </c>
-      <c r="J10">
+      <c r="J15">
         <v>863554</v>
       </c>
-      <c r="K10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L10">
+      <c r="K15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15">
         <f t="shared" si="0"/>
         <v>5.9362895001765024</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N15" t="s">
         <v>24</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O15" t="s">
         <v>25</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P15" t="s">
         <v>26</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q15" t="s">
         <v>27</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
-      <c r="C12" s="3" t="s">
+    <row r="17" spans="3:19">
+      <c r="C17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="F12" t="s">
+      <c r="D17" s="3"/>
+      <c r="F17" t="s">
         <v>5</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
-      <c r="G13" t="s">
+    <row r="18" spans="3:19">
+      <c r="G18" t="s">
         <v>7</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H18" t="s">
         <v>8</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I18" t="s">
         <v>9</v>
       </c>
-      <c r="J13">
+      <c r="J18">
         <v>15640</v>
       </c>
-      <c r="K13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L13">
-        <f t="shared" ref="L13:L19" si="1">+LOG(J13)</f>
+      <c r="K18" t="s">
+        <v>10</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ref="L18:L24" si="1">+LOG(J18)</f>
         <v>4.1942367487238288</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
-      <c r="G14" t="s">
+    <row r="19" spans="3:19">
+      <c r="G19" t="s">
         <v>7</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H19" t="s">
         <v>11</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I19" t="s">
         <v>9</v>
       </c>
-      <c r="J14">
+      <c r="J19">
         <v>25576</v>
       </c>
-      <c r="K14" t="s">
-        <v>10</v>
-      </c>
-      <c r="L14">
+      <c r="K19" t="s">
+        <v>10</v>
+      </c>
+      <c r="L19">
         <f t="shared" si="1"/>
         <v>4.4078326232636318</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
-      <c r="F15" t="s">
+    <row r="20" spans="3:19">
+      <c r="F20" t="s">
         <v>12</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G20" t="s">
         <v>13</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H20" t="s">
         <v>14</v>
       </c>
-      <c r="J15">
+      <c r="J20">
         <v>41216</v>
       </c>
-      <c r="K15" t="s">
-        <v>10</v>
-      </c>
-      <c r="L15">
+      <c r="K20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L20">
         <f t="shared" si="1"/>
         <v>4.6150658413436991</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N20" t="s">
         <v>15</v>
       </c>
-      <c r="O15">
+      <c r="O20">
         <v>83364</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P20" t="s">
         <v>16</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="Q20" s="1">
         <v>0.33100000000000002</v>
       </c>
-      <c r="R15" t="s">
+      <c r="R20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
-      <c r="F16" t="s">
+    <row r="21" spans="3:19">
+      <c r="F21" t="s">
         <v>12</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G21" t="s">
         <v>13</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H21" t="s">
         <v>18</v>
       </c>
-      <c r="J16">
+      <c r="J21">
         <v>114907</v>
       </c>
-      <c r="K16" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16">
+      <c r="K21" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21">
         <f t="shared" si="1"/>
         <v>5.0603464862058916</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N21" t="s">
         <v>15</v>
       </c>
-      <c r="O16">
+      <c r="O21">
         <v>16165</v>
       </c>
-      <c r="P16" t="s">
+      <c r="P21" t="s">
         <v>16</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="Q21" s="1">
         <v>0.877</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R21" t="s">
         <v>17</v>
       </c>
-      <c r="S16" t="s">
+      <c r="S21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="6:18">
-      <c r="G17" t="s">
+    <row r="22" spans="3:19">
+      <c r="G22" t="s">
         <v>19</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H22" t="s">
         <v>20</v>
       </c>
-      <c r="J17">
+      <c r="J22">
         <v>599399</v>
       </c>
-      <c r="K17" t="s">
-        <v>10</v>
-      </c>
-      <c r="L17">
+      <c r="K22" t="s">
+        <v>10</v>
+      </c>
+      <c r="L22">
         <f t="shared" si="1"/>
         <v>5.7777160140603367</v>
       </c>
     </row>
-    <row r="18" spans="6:18">
-      <c r="G18" t="s">
+    <row r="23" spans="3:19">
+      <c r="G23" t="s">
         <v>19</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H23" t="s">
         <v>21</v>
       </c>
-      <c r="J18">
+      <c r="J23">
         <v>108032</v>
       </c>
-      <c r="K18" t="s">
-        <v>10</v>
-      </c>
-      <c r="L18">
+      <c r="K23" t="s">
+        <v>10</v>
+      </c>
+      <c r="L23">
         <f t="shared" si="1"/>
         <v>5.0335524162735235</v>
       </c>
     </row>
-    <row r="19" spans="6:18">
-      <c r="F19" t="s">
+    <row r="24" spans="3:19">
+      <c r="F24" t="s">
         <v>5</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G24" t="s">
         <v>22</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H24" t="s">
         <v>23</v>
       </c>
-      <c r="J19">
+      <c r="J24">
         <v>863554</v>
       </c>
-      <c r="K19" t="s">
-        <v>10</v>
-      </c>
-      <c r="L19">
+      <c r="K24" t="s">
+        <v>10</v>
+      </c>
+      <c r="L24">
         <f t="shared" si="1"/>
         <v>5.9362895001765024</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N24" t="s">
         <v>24</v>
       </c>
-      <c r="O19" t="s">
+      <c r="O24" t="s">
         <v>25</v>
       </c>
-      <c r="P19" t="s">
+      <c r="P24" t="s">
         <v>26</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="Q24" t="s">
         <v>27</v>
       </c>
-      <c r="R19" t="s">
+      <c r="R24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="6:18">
-      <c r="F21" s="2" t="s">
+    <row r="26" spans="3:19">
+      <c r="F26" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-    </row>
-    <row r="23" spans="6:18">
-      <c r="F23" t="s">
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+    </row>
+    <row r="28" spans="3:19">
+      <c r="F28" t="s">
         <v>5</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="6:18">
-      <c r="G24" t="s">
+    <row r="29" spans="3:19">
+      <c r="G29" t="s">
         <v>7</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H29" t="s">
         <v>8</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I29" t="s">
         <v>9</v>
       </c>
-      <c r="J24">
+      <c r="J29">
         <v>13376</v>
       </c>
-      <c r="K24" t="s">
-        <v>10</v>
-      </c>
-      <c r="L24">
-        <f t="shared" ref="L24:L30" si="2">+LOG(J24)</f>
+      <c r="K29" t="s">
+        <v>10</v>
+      </c>
+      <c r="L29">
+        <f t="shared" ref="L29:L35" si="2">+LOG(J29)</f>
         <v>4.1263262600949409</v>
       </c>
     </row>
-    <row r="25" spans="6:18">
-      <c r="G25" t="s">
+    <row r="30" spans="3:19">
+      <c r="G30" t="s">
         <v>7</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H30" t="s">
         <v>11</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I30" t="s">
         <v>9</v>
       </c>
-      <c r="J25">
+      <c r="J30">
         <v>27896</v>
       </c>
-      <c r="K25" t="s">
-        <v>10</v>
-      </c>
-      <c r="L25">
+      <c r="K30" t="s">
+        <v>10</v>
+      </c>
+      <c r="L30">
         <f t="shared" si="2"/>
         <v>4.4455419343679203</v>
       </c>
     </row>
-    <row r="26" spans="6:18">
-      <c r="F26" t="s">
+    <row r="31" spans="3:19">
+      <c r="F31" t="s">
         <v>12</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G31" t="s">
         <v>13</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H31" t="s">
         <v>14</v>
       </c>
-      <c r="J26">
+      <c r="J31">
         <v>41272</v>
       </c>
-      <c r="K26" t="s">
-        <v>10</v>
-      </c>
-      <c r="L26">
+      <c r="K31" t="s">
+        <v>10</v>
+      </c>
+      <c r="L31">
         <f t="shared" si="2"/>
         <v>4.6156555148652521</v>
       </c>
-      <c r="N26" t="s">
+      <c r="N31" t="s">
         <v>15</v>
       </c>
-      <c r="O26">
+      <c r="O31">
         <v>83308</v>
       </c>
-      <c r="P26" t="s">
+      <c r="P31" t="s">
         <v>16</v>
       </c>
-      <c r="Q26" s="1">
+      <c r="Q31" s="1">
         <v>0.33100000000000002</v>
       </c>
-      <c r="R26" t="s">
+      <c r="R31" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="6:18">
-      <c r="F27" t="s">
+    <row r="32" spans="3:19">
+      <c r="F32" t="s">
         <v>12</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G32" t="s">
         <v>13</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H32" t="s">
         <v>18</v>
       </c>
-      <c r="J27">
+      <c r="J32">
         <v>90911</v>
       </c>
-      <c r="K27" t="s">
-        <v>10</v>
-      </c>
-      <c r="L27">
+      <c r="K32" t="s">
+        <v>10</v>
+      </c>
+      <c r="L32">
         <f t="shared" si="2"/>
         <v>4.9586164349301347</v>
       </c>
-      <c r="N27" t="s">
+      <c r="N32" t="s">
         <v>15</v>
       </c>
-      <c r="O27">
+      <c r="O32">
         <v>40161</v>
       </c>
-      <c r="P27" t="s">
+      <c r="P32" t="s">
         <v>16</v>
       </c>
-      <c r="Q27" s="1">
+      <c r="Q32" s="1">
         <v>0.69399999999999995</v>
       </c>
-      <c r="R27" t="s">
+      <c r="R32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="6:18">
-      <c r="G28" t="s">
+    <row r="33" spans="2:18">
+      <c r="G33" t="s">
         <v>19</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H33" t="s">
         <v>20</v>
       </c>
-      <c r="J28">
+      <c r="J33">
         <v>616011</v>
       </c>
-      <c r="K28" t="s">
-        <v>10</v>
-      </c>
-      <c r="L28">
+      <c r="K33" t="s">
+        <v>10</v>
+      </c>
+      <c r="L33">
         <f t="shared" si="2"/>
         <v>5.7895884673537887</v>
       </c>
     </row>
-    <row r="29" spans="6:18">
-      <c r="G29" t="s">
+    <row r="34" spans="2:18">
+      <c r="G34" t="s">
         <v>19</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H34" t="s">
         <v>21</v>
       </c>
-      <c r="J29">
+      <c r="J34">
         <v>153336</v>
       </c>
-      <c r="K29" t="s">
-        <v>10</v>
-      </c>
-      <c r="L29">
+      <c r="K34" t="s">
+        <v>10</v>
+      </c>
+      <c r="L34">
         <f t="shared" si="2"/>
         <v>5.1856441298437463</v>
       </c>
     </row>
-    <row r="30" spans="6:18">
-      <c r="F30" t="s">
+    <row r="35" spans="2:18">
+      <c r="F35" t="s">
         <v>5</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G35" t="s">
         <v>22</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H35" t="s">
         <v>23</v>
       </c>
-      <c r="J30">
+      <c r="J35">
         <v>901530</v>
       </c>
-      <c r="K30" t="s">
-        <v>10</v>
-      </c>
-      <c r="L30">
+      <c r="K35" t="s">
+        <v>10</v>
+      </c>
+      <c r="L35">
         <f t="shared" si="2"/>
         <v>5.9549801832133582</v>
       </c>
-      <c r="N30" t="s">
+      <c r="N35" t="s">
         <v>24</v>
       </c>
-      <c r="O30" t="s">
+      <c r="O35" t="s">
         <v>25</v>
       </c>
-      <c r="P30" t="s">
+      <c r="P35" t="s">
         <v>26</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="Q35" t="s">
         <v>27</v>
       </c>
-      <c r="R30" t="s">
+      <c r="R35" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18">
+      <c r="D38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18">
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18">
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18">
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18">
+      <c r="F44" t="s">
+        <v>5</v>
+      </c>
+      <c r="G44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18">
+      <c r="F45" s="7"/>
+      <c r="G45" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" t="s">
+        <v>8</v>
+      </c>
+      <c r="I45" t="s">
+        <v>9</v>
+      </c>
+      <c r="J45">
+        <v>15424</v>
+      </c>
+      <c r="K45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18">
+      <c r="G46" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" t="s">
+        <v>9</v>
+      </c>
+      <c r="J46">
+        <v>31208</v>
+      </c>
+      <c r="K46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="2:18">
+      <c r="F47" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" t="s">
+        <v>14</v>
+      </c>
+      <c r="J47">
+        <v>46632</v>
+      </c>
+      <c r="K47" t="s">
+        <v>10</v>
+      </c>
+      <c r="M47" t="s">
+        <v>15</v>
+      </c>
+      <c r="N47">
+        <v>77948</v>
+      </c>
+      <c r="O47" t="s">
+        <v>16</v>
+      </c>
+      <c r="P47" s="1">
+        <v>0.374</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="2:18">
+      <c r="F48" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" t="s">
+        <v>18</v>
+      </c>
+      <c r="J48">
+        <v>113759</v>
+      </c>
+      <c r="K48" t="s">
+        <v>10</v>
+      </c>
+      <c r="M48" t="s">
+        <v>15</v>
+      </c>
+      <c r="N48">
+        <v>17313</v>
+      </c>
+      <c r="O48" t="s">
+        <v>16</v>
+      </c>
+      <c r="P48" s="1">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="6:17">
+      <c r="G49" t="s">
+        <v>19</v>
+      </c>
+      <c r="H49" t="s">
+        <v>20</v>
+      </c>
+      <c r="J49">
+        <v>677739</v>
+      </c>
+      <c r="K49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="6:17">
+      <c r="G50" t="s">
+        <v>19</v>
+      </c>
+      <c r="H50" t="s">
+        <v>21</v>
+      </c>
+      <c r="J50">
+        <v>156976</v>
+      </c>
+      <c r="K50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="6:17">
+      <c r="F51" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" t="s">
+        <v>22</v>
+      </c>
+      <c r="H51" t="s">
+        <v>23</v>
+      </c>
+      <c r="J51">
+        <v>995106</v>
+      </c>
+      <c r="K51" t="s">
+        <v>10</v>
+      </c>
+      <c r="M51" t="s">
+        <v>24</v>
+      </c>
+      <c r="N51" t="s">
+        <v>25</v>
+      </c>
+      <c r="O51" t="s">
+        <v>26</v>
+      </c>
+      <c r="P51" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="6:17">
+      <c r="J54">
+        <v>1048576</v>
+      </c>
+    </row>
+    <row r="56" spans="6:17">
+      <c r="J56">
+        <f>+J54-J51</f>
+        <v>53470</v>
+      </c>
+      <c r="K56">
+        <f>+J56/J54</f>
+        <v>5.0992965698242188E-2</v>
+      </c>
+      <c r="L56" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>